<commit_message>
Delta - Travel Update Center Page - 6 Test Cases Done
</commit_message>
<xml_diff>
--- a/deltaAirlines/src/main/resources/DeltaTravelUpdateCenterPage_ExpectedElements.xlsx
+++ b/deltaAirlines/src/main/resources/DeltaTravelUpdateCenterPage_ExpectedElements.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Page URL" sheetId="1" r:id="rId1"/>
     <sheet name="TUC Dropdown List Count" sheetId="2" r:id="rId2"/>
     <sheet name="TUC Dropdown List Names" sheetId="3" r:id="rId3"/>
     <sheet name="TUC - WWKYS Submenu Names" sheetId="4" r:id="rId4"/>
+    <sheet name="TUC - FDTOC Submenu Names" sheetId="5" r:id="rId5"/>
+    <sheet name="TUC - FWYNTK Submenu Names" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>https://www.delta.com/us/en/travel-update-center/overview</t>
   </si>
@@ -75,6 +77,21 @@
   </si>
   <si>
     <t>Temperature Screening at Delta Facilities</t>
+  </si>
+  <si>
+    <t>Weekly Update from CEO Ed Bastian</t>
+  </si>
+  <si>
+    <t>How Delta is Supporting Medical Volunteers</t>
+  </si>
+  <si>
+    <t>Coronavirus Regional Restrictions</t>
+  </si>
+  <si>
+    <t>Delta Temporarily Closes Select Airports</t>
+  </si>
+  <si>
+    <t>Things to Know When You Travel with a Partner Airline</t>
   </si>
 </sst>
 </file>
@@ -492,9 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -539,4 +554,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Delta - Travel Update Center Page - 13 Test Cases Done
</commit_message>
<xml_diff>
--- a/deltaAirlines/src/main/resources/DeltaTravelUpdateCenterPage_ExpectedElements.xlsx
+++ b/deltaAirlines/src/main/resources/DeltaTravelUpdateCenterPage_ExpectedElements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Page URL" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,13 @@
     <sheet name="TUC - WWKYS Submenu Names" sheetId="4" r:id="rId4"/>
     <sheet name="TUC - FDTOC Submenu Names" sheetId="5" r:id="rId5"/>
     <sheet name="TUC - FWYNTK Submenu Names" sheetId="6" r:id="rId6"/>
+    <sheet name="CUC - Grid Header Names" sheetId="7" r:id="rId7"/>
+    <sheet name="CUC - TravelFlexibility Names" sheetId="8" r:id="rId8"/>
+    <sheet name="CUC - TravelFlexibility URLs" sheetId="12" r:id="rId9"/>
+    <sheet name="CUC - TravelingWithUs Names" sheetId="9" r:id="rId10"/>
+    <sheet name="CUC - TravelingWithUs URLs" sheetId="13" r:id="rId11"/>
+    <sheet name="CUC - CaringForYou Names" sheetId="10" r:id="rId12"/>
+    <sheet name="CUC - CaringForYou URLs" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>https://www.delta.com/us/en/travel-update-center/overview</t>
   </si>
@@ -92,6 +99,75 @@
   </si>
   <si>
     <t>Things to Know When You Travel with a Partner Airline</t>
+  </si>
+  <si>
+    <t>TRAVEL FLEXIBILITY</t>
+  </si>
+  <si>
+    <t>TRAVELING WITH US</t>
+  </si>
+  <si>
+    <t>CARING FOR YOU</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/overview#waiver</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/overview#confidence</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/overview#faq</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/overview#deltaclean</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/overview#skyclub</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/overview#flydeltaapp</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/overview#skymiles</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/overview#frontlines</t>
+  </si>
+  <si>
+    <t>Updates, Waivers and eCredits
+, Go to footer note</t>
+  </si>
+  <si>
+    <t>Booking with Confidence
+, Go to footer note</t>
+  </si>
+  <si>
+    <t>Frequently Asked Questions
+, Go to footer note</t>
+  </si>
+  <si>
+    <t>Standard for Safer Travel
+, Go to footer note</t>
+  </si>
+  <si>
+    <t>SkyMiles® Program Updates
+, Go to footer note</t>
+  </si>
+  <si>
+    <t>Supporting Medical Volunteers
+, Go to footer note</t>
+  </si>
+  <si>
+    <t>Protective Equipment for Healthcare Workers
+, Go to footer note</t>
+  </si>
+  <si>
+    <t>Delta Sky Club Updates
+, Go to footer note</t>
+  </si>
+  <si>
+    <t>Download the Fly Delta App
+, Go to footer note</t>
   </si>
 </sst>
 </file>
@@ -127,8 +203,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,6 +508,138 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D6:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -583,7 +794,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -605,4 +818,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D7:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Delta - Travel Update Center Page - 20 Test Cases (COMPLETE)
</commit_message>
<xml_diff>
--- a/deltaAirlines/src/main/resources/DeltaTravelUpdateCenterPage_ExpectedElements.xlsx
+++ b/deltaAirlines/src/main/resources/DeltaTravelUpdateCenterPage_ExpectedElements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="16" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Page URL" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,12 @@
     <sheet name="CUC - TravelingWithUs URLs" sheetId="13" r:id="rId11"/>
     <sheet name="CUC - CaringForYou Names" sheetId="10" r:id="rId12"/>
     <sheet name="CUC - CaringForYou URLs" sheetId="14" r:id="rId13"/>
+    <sheet name="SACRU - URLs" sheetId="15" r:id="rId14"/>
+    <sheet name="OUATT - Header Names" sheetId="16" r:id="rId15"/>
+    <sheet name="OUATT - DeltaSkyClub URL" sheetId="17" r:id="rId16"/>
+    <sheet name="OUATT - FlyDeltaApp URL" sheetId="18" r:id="rId17"/>
+    <sheet name="OUATT - FlyingPartnerAir URL" sheetId="20" r:id="rId18"/>
+    <sheet name="FAQ Header Names" sheetId="21" r:id="rId19"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>https://www.delta.com/us/en/travel-update-center/overview</t>
   </si>
@@ -168,6 +174,60 @@
   <si>
     <t>Download the Fly Delta App
 , Go to footer note</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/extending-skymiles-benefits?src=benefits3</t>
+  </si>
+  <si>
+    <t>http://amex.co/extrasupport?src=amex3</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/ways-we-are-keeping-you-safe/onboard-services?src=obsspace1#socialdist</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/skymiles/program-resources/news-and-updates?src=sm1a#recent</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/extending-skymiles-benefits?src=benefits1</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/ways-we-are-keeping-you-safe/onboard-services?src=obs1</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/flying-what-you-need-to-know/coronavirus-regional-restrictions?src=restrictions1</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/from-delta-to-our-customers/medical-volunteers-book-free?src=flyfree1</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/delta-digital/mobile?src=app1</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/coronavirus-update-center/ways-we-are-keeping-you-safe/skyclub-update?src=skyclub1</t>
+  </si>
+  <si>
+    <t>DOWNLOAD THE FLY DELTA APP</t>
+  </si>
+  <si>
+    <t>FLYING WITH A PARTNER AIRLINE?</t>
+  </si>
+  <si>
+    <t>DELTA SKY CLUB UPDATES</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/ways-we-are-keeping-you-safe/skyclub-update</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/delta-digital/mobile?src=app2</t>
+  </si>
+  <si>
+    <t>https://www.delta.com/us/en/travel-update-center/flying-what-you-need-to-know/things-to-know-when-you-travel-with-a-partner-airline</t>
+  </si>
+  <si>
+    <t>SAFER TRAVEL</t>
+  </si>
+  <si>
+    <t>DELTA PARTNERS AND AFFILIATES</t>
   </si>
 </sst>
 </file>
@@ -512,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -640,6 +700,201 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="125.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="93.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
new helper Assert methods in WebAPI + re-structured Delta
</commit_message>
<xml_diff>
--- a/deltaAirlines/src/main/resources/DeltaTravelUpdateCenterPage_ExpectedElements.xlsx
+++ b/deltaAirlines/src/main/resources/DeltaTravelUpdateCenterPage_ExpectedElements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="16" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Page URL" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="CUC - TravelingWithUs URLs" sheetId="13" r:id="rId11"/>
     <sheet name="CUC - CaringForYou Names" sheetId="10" r:id="rId12"/>
     <sheet name="CUC - CaringForYou URLs" sheetId="14" r:id="rId13"/>
-    <sheet name="SACRU - URLs" sheetId="15" r:id="rId14"/>
+    <sheet name="SARCU - URLs" sheetId="15" r:id="rId14"/>
     <sheet name="OUATT - Header Names" sheetId="16" r:id="rId15"/>
     <sheet name="OUATT - DeltaSkyClub URL" sheetId="17" r:id="rId16"/>
     <sheet name="OUATT - FlyDeltaApp URL" sheetId="18" r:id="rId17"/>
@@ -704,7 +704,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -851,6 +853,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="130.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -866,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -899,7 +904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>